<commit_message>
docs: results and data
</commit_message>
<xml_diff>
--- a/results/CIT.xlsx
+++ b/results/CIT.xlsx
@@ -544,7 +544,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>0.1204325429604989</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -553,7 +553,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>0.2874501708223065</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -583,7 +583,7 @@
         <v>0</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <v>0.5921172862171945</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -710,7 +710,7 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <v>0.4406500996151126</v>
+        <v>0</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -781,13 +781,13 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>0.9492480771877249</v>
+        <v>0</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6">
-        <v>0.5101026577201669</v>
+        <v>0</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -826,7 +826,7 @@
         <v>0</v>
       </c>
       <c r="X6">
-        <v>0.1287728355876866</v>
+        <v>0</v>
       </c>
       <c r="Y6">
         <v>0</v>
@@ -840,7 +840,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>0.1204325429604989</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -855,22 +855,22 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0.09475633363640217</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>0.05075192281227514</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7">
-        <v>0.03717187094160868</v>
+        <v>0</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>0.1003814589172418</v>
+        <v>0</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -882,13 +882,13 @@
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>0.1123218570984662</v>
+        <v>0</v>
       </c>
       <c r="R7">
         <v>0</v>
       </c>
       <c r="S7">
-        <v>0.06163052902152446</v>
+        <v>0</v>
       </c>
       <c r="T7">
         <v>0</v>
@@ -903,7 +903,7 @@
         <v>0</v>
       </c>
       <c r="X7">
-        <v>0.05347445417152326</v>
+        <v>0</v>
       </c>
       <c r="Y7">
         <v>0</v>
@@ -929,7 +929,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>0.09475633363640217</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -938,7 +938,7 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>0.8675622404910103</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -953,7 +953,7 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>0</v>
+        <v>0.03768142587258756</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -1003,10 +1003,10 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>0.9492480771877249</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>0.05075192281227514</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1071,7 +1071,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>0.2874501708223065</v>
+        <v>0</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1086,7 +1086,7 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>0.8675622404910103</v>
+        <v>0</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -1101,7 +1101,7 @@
         <v>0</v>
       </c>
       <c r="M10">
-        <v>0.2714521275478711</v>
+        <v>0</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -1113,13 +1113,13 @@
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>0.2543759704877028</v>
+        <v>0</v>
       </c>
       <c r="R10">
         <v>0</v>
       </c>
       <c r="S10">
-        <v>0.1395750216075701</v>
+        <v>0</v>
       </c>
       <c r="T10">
         <v>0</v>
@@ -1134,10 +1134,10 @@
         <v>0</v>
       </c>
       <c r="X10">
-        <v>0.3990366189573973</v>
+        <v>0</v>
       </c>
       <c r="Y10">
-        <v>0.8870902668099052</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1154,13 +1154,13 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>0.4406500996151126</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>0.5101026577201669</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>0.03717187094160868</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1199,7 +1199,7 @@
         <v>0</v>
       </c>
       <c r="T11">
-        <v>0</v>
+        <v>0.01207537172311179</v>
       </c>
       <c r="U11">
         <v>0</v>
@@ -1261,7 +1261,7 @@
         <v>0</v>
       </c>
       <c r="O12">
-        <v>0</v>
+        <v>0.08433330658934152</v>
       </c>
       <c r="P12">
         <v>0</v>
@@ -1276,10 +1276,10 @@
         <v>0</v>
       </c>
       <c r="T12">
-        <v>0</v>
+        <v>0.5367373836391109</v>
       </c>
       <c r="U12">
-        <v>0</v>
+        <v>0.3789293097715476</v>
       </c>
       <c r="V12">
         <v>0</v>
@@ -1314,7 +1314,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>0.1003814589172418</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1323,7 +1323,7 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>0.2714521275478711</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -1353,7 +1353,7 @@
         <v>0</v>
       </c>
       <c r="T13">
-        <v>0</v>
+        <v>0.6281664135348871</v>
       </c>
       <c r="U13">
         <v>0</v>
@@ -1471,7 +1471,7 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <v>0.03768142587258756</v>
+        <v>0</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -1483,7 +1483,7 @@
         <v>0</v>
       </c>
       <c r="L15">
-        <v>0.08433330658934159</v>
+        <v>0</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -1501,7 +1501,7 @@
         <v>0</v>
       </c>
       <c r="R15">
-        <v>0.2437926068535217</v>
+        <v>0</v>
       </c>
       <c r="S15">
         <v>0</v>
@@ -1522,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="Y15">
-        <v>0.1129097331900948</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -1622,7 +1622,7 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>0.1123218570984662</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -1631,7 +1631,7 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>0.2543759704877028</v>
       </c>
       <c r="K17">
         <v>0</v>
@@ -1661,7 +1661,7 @@
         <v>0</v>
       </c>
       <c r="T17">
-        <v>0</v>
+        <v>0.633302172413831</v>
       </c>
       <c r="U17">
         <v>0</v>
@@ -1723,7 +1723,7 @@
         <v>0</v>
       </c>
       <c r="O18">
-        <v>0</v>
+        <v>0.2437926068535217</v>
       </c>
       <c r="P18">
         <v>0</v>
@@ -1738,10 +1738,10 @@
         <v>0</v>
       </c>
       <c r="T18">
-        <v>0</v>
+        <v>0.4756442191313157</v>
       </c>
       <c r="U18">
-        <v>0</v>
+        <v>0.2805631740151626</v>
       </c>
       <c r="V18">
         <v>0</v>
@@ -1776,7 +1776,7 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>0.06163052902152446</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1785,7 +1785,7 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>0.1395750216075701</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -1815,7 +1815,7 @@
         <v>0</v>
       </c>
       <c r="T19">
-        <v>0</v>
+        <v>0.7987944493709055</v>
       </c>
       <c r="U19">
         <v>0</v>
@@ -1841,7 +1841,7 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <v>0.5921172862171945</v>
+        <v>0</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1865,13 +1865,13 @@
         <v>0</v>
       </c>
       <c r="K20">
-        <v>0.01207537172311179</v>
+        <v>0</v>
       </c>
       <c r="L20">
-        <v>0.5367373836391109</v>
+        <v>0</v>
       </c>
       <c r="M20">
-        <v>0.6281664135348871</v>
+        <v>0</v>
       </c>
       <c r="N20">
         <v>0</v>
@@ -1883,13 +1883,13 @@
         <v>0</v>
       </c>
       <c r="Q20">
-        <v>0.633302172413831</v>
+        <v>0</v>
       </c>
       <c r="R20">
-        <v>0.4756442191313155</v>
+        <v>0</v>
       </c>
       <c r="S20">
-        <v>0.7987944493709055</v>
+        <v>0</v>
       </c>
       <c r="T20">
         <v>1</v>
@@ -1904,7 +1904,7 @@
         <v>0</v>
       </c>
       <c r="X20">
-        <v>0.4187160912833928</v>
+        <v>0</v>
       </c>
       <c r="Y20">
         <v>0</v>
@@ -1945,7 +1945,7 @@
         <v>0</v>
       </c>
       <c r="L21">
-        <v>0.3789293097715475</v>
+        <v>0</v>
       </c>
       <c r="M21">
         <v>0</v>
@@ -1963,7 +1963,7 @@
         <v>0</v>
       </c>
       <c r="R21">
-        <v>0.2805631740151628</v>
+        <v>0</v>
       </c>
       <c r="S21">
         <v>0</v>
@@ -2158,10 +2158,10 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>0.1287728355876866</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>0.05347445417152326</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -2170,7 +2170,7 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>0.3990366189573973</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -2200,7 +2200,7 @@
         <v>0</v>
       </c>
       <c r="T24">
-        <v>0</v>
+        <v>0.4187160912833928</v>
       </c>
       <c r="U24">
         <v>0</v>
@@ -2247,7 +2247,7 @@
         <v>0</v>
       </c>
       <c r="J25">
-        <v>0</v>
+        <v>0.8870902668099052</v>
       </c>
       <c r="K25">
         <v>0</v>
@@ -2262,7 +2262,7 @@
         <v>0</v>
       </c>
       <c r="O25">
-        <v>0</v>
+        <v>0.1129097331900948</v>
       </c>
       <c r="P25">
         <v>0</v>
@@ -2387,76 +2387,76 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>0.6599006090483395</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>0.7003871909813109</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.03009285297811815</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>0.2870887548328691</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>0.973185466738121</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>0.04313588915212152</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>0.9631175070227463</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>0.03278614440816596</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>0.9012589160324767</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>0.6579942322400196</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>0.8150927473684779</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>0.4015376883739908</v>
       </c>
       <c r="P2">
-        <v>0.5778522339386156</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>0.6468546256285614</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>0.9985062376000774</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>0.6077264995218093</v>
+        <v>0.5984623116260092</v>
       </c>
       <c r="T2">
-        <v>0.5601545142717921</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>0.6026295548080869</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>0.8334069326097517</v>
+        <v>0</v>
       </c>
       <c r="W2">
-        <v>0.1439498693142103</v>
+        <v>0</v>
       </c>
       <c r="X2">
-        <v>0.6614140197534236</v>
+        <v>0</v>
       </c>
       <c r="Y2">
-        <v>0.8543721662740987</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -2464,7 +2464,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.6599006090483395</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -2473,7 +2473,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.3400993909516606</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2580,7 +2580,7 @@
         <v>0</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>0.5808446626520776</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -2592,7 +2592,7 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>0.4191553373479224</v>
       </c>
       <c r="T4">
         <v>0</v>
@@ -2621,7 +2621,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>0.3400993909516606</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -2630,61 +2630,61 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0.9699071470218819</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>0.7129112451671309</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>0.02681453326187897</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>0.9568641108478785</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5">
-        <v>0.967213855591834</v>
+        <v>0</v>
       </c>
       <c r="L5">
-        <v>0.09874108396752337</v>
+        <v>0</v>
       </c>
       <c r="M5">
-        <v>0.3420057677599804</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>0.1849072526315221</v>
+        <v>0</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0.4221477660613844</v>
+        <v>0</v>
       </c>
       <c r="Q5">
-        <v>0.3531453743714386</v>
+        <v>0</v>
       </c>
       <c r="R5">
-        <v>0.001493762399922614</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>0.3922735004781907</v>
+        <v>0</v>
       </c>
       <c r="T5">
-        <v>0.4398454857282079</v>
+        <v>0</v>
       </c>
       <c r="U5">
         <v>0</v>
       </c>
       <c r="V5">
-        <v>0.1665930673902483</v>
+        <v>0</v>
       </c>
       <c r="W5">
-        <v>0.8560501306857897</v>
+        <v>0</v>
       </c>
       <c r="X5">
-        <v>0.3385859802465764</v>
+        <v>0</v>
       </c>
       <c r="Y5">
         <v>0</v>
@@ -2695,7 +2695,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>0.03009285297811815</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -2704,7 +2704,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>0.9699071470218819</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -2772,7 +2772,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>0.2870887548328691</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -2781,7 +2781,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.7129112451671309</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -2849,7 +2849,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>0.973185466738121</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -2858,7 +2858,7 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.02681453326187897</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -2926,7 +2926,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>0.04313588915212152</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -2935,7 +2935,7 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.9568641108478785</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -3042,7 +3042,7 @@
         <v>0</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <v>0.4236104703796881</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -3054,7 +3054,7 @@
         <v>0</v>
       </c>
       <c r="S10">
-        <v>0</v>
+        <v>0.5763895296203119</v>
       </c>
       <c r="T10">
         <v>0</v>
@@ -3080,7 +3080,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>0.03278614440816596</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -3089,7 +3089,7 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>0.967213855591834</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -3157,7 +3157,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>0.9012589160324767</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -3166,7 +3166,7 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.09874108396752337</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -3234,7 +3234,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>0.6579942322400196</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -3243,7 +3243,7 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>0.3420057677599804</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -3311,7 +3311,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>0.8150927473684779</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -3320,7 +3320,7 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>0.1849072526315221</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -3394,7 +3394,7 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>0.2996128090186891</v>
+        <v>0</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -3412,7 +3412,7 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>0.03688249297725369</v>
+        <v>0</v>
       </c>
       <c r="K15">
         <v>0</v>
@@ -3445,7 +3445,7 @@
         <v>0</v>
       </c>
       <c r="U15">
-        <v>0.3973704451919131</v>
+        <v>0</v>
       </c>
       <c r="V15">
         <v>0</v>
@@ -3457,7 +3457,7 @@
         <v>0</v>
       </c>
       <c r="Y15">
-        <v>0.1456278337259012</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -3465,7 +3465,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>0.5778522339386156</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -3474,7 +3474,7 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>0.4221477660613844</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -3542,7 +3542,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>0.6468546256285614</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -3551,7 +3551,7 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>0.3531453743714386</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -3619,7 +3619,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>0.9985062376000774</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -3628,7 +3628,7 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>0.001493762399922614</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -3696,7 +3696,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>0.6077264995218093</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -3705,7 +3705,7 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>0.3922735004781907</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -3773,7 +3773,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>0.5601545142717921</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -3782,7 +3782,7 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>0.4398454857282079</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -3850,7 +3850,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>0.2861161368141096</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -3889,7 +3889,7 @@
         <v>0</v>
       </c>
       <c r="O21">
-        <v>0</v>
+        <v>0.5244625113925655</v>
       </c>
       <c r="P21">
         <v>0</v>
@@ -3901,7 +3901,7 @@
         <v>0</v>
       </c>
       <c r="S21">
-        <v>0</v>
+        <v>0.1894213517933249</v>
       </c>
       <c r="T21">
         <v>0</v>
@@ -3927,7 +3927,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>0.8334069326097517</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -3936,7 +3936,7 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>0.1665930673902483</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -4004,7 +4004,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>0.1439498693142103</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -4013,7 +4013,7 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>0.8560501306857897</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -4081,7 +4081,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>0.6614140197534236</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -4090,7 +4090,7 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>0.3385859802465764</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -4197,7 +4197,7 @@
         <v>0</v>
       </c>
       <c r="O25">
-        <v>0</v>
+        <v>0.4886904583826819</v>
       </c>
       <c r="P25">
         <v>0</v>
@@ -4209,7 +4209,7 @@
         <v>0</v>
       </c>
       <c r="S25">
-        <v>0</v>
+        <v>0.5113095416173181</v>
       </c>
       <c r="T25">
         <v>0</v>

</xml_diff>